<commit_message>
updating daily progress in Spread sheet
</commit_message>
<xml_diff>
--- a/Master-Sheet.xlsx
+++ b/Master-Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OTHERS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF013AD0-B671-483B-AC03-671DA639B1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E70A352-C8A6-4155-BE87-F67C6A5C6945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="702" xr2:uid="{0042A21B-FF33-4EBF-B65C-49274797135A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="702" activeTab="1" xr2:uid="{0042A21B-FF33-4EBF-B65C-49274797135A}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily" sheetId="10" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="132">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -129,9 +129,6 @@
     <t>Leetcode Questions  ( Total = 0 )</t>
   </si>
   <si>
-    <t>Geeksforgeeks Questions ( Total = 0 )</t>
-  </si>
-  <si>
     <t>Coding contests ( Total = 0 )</t>
   </si>
   <si>
@@ -261,9 +258,6 @@
     <t xml:space="preserve">Propositions and 1st order logic - DM </t>
   </si>
   <si>
-    <t>Qs of Array on GFG &amp; Leetcode</t>
-  </si>
-  <si>
     <t>Complete 10 points on Arcade</t>
   </si>
   <si>
@@ -373,13 +367,76 @@
   </si>
   <si>
     <t>Complete the Projects said by Love Babbar</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Qs of Array on GFG</t>
+  </si>
+  <si>
+    <t>Missing in Array</t>
+  </si>
+  <si>
+    <t>Array</t>
+  </si>
+  <si>
+    <t>Array Duplicates</t>
+  </si>
+  <si>
+    <t>Wave Array</t>
+  </si>
+  <si>
+    <t>Implement 2 stacks in single array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Queue reversal </t>
+  </si>
+  <si>
+    <t>Summed matrix</t>
+  </si>
+  <si>
+    <t>Geeksforgeeks Questions ( Total = 6)</t>
+  </si>
+  <si>
+    <t>Two Sum</t>
+  </si>
+  <si>
+    <t>Reverse integer</t>
+  </si>
+  <si>
+    <t>Palindrome number</t>
+  </si>
+  <si>
+    <t>Remove Duplicates from sorted Array</t>
+  </si>
+  <si>
+    <t>Complement of base 10 integer</t>
+  </si>
+  <si>
+    <t># successful submissions</t>
+  </si>
+  <si>
+    <t>Problem No.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 // 1 </t>
+  </si>
+  <si>
+    <t>1 // 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 // 2 </t>
+  </si>
+  <si>
+    <t>Basic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -471,6 +528,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -516,7 +580,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -537,32 +601,39 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="101">
+  <dxfs count="100">
     <dxf>
       <fill>
         <patternFill>
@@ -640,19 +711,18 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -675,117 +745,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -823,15 +782,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -860,9 +810,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -894,9 +841,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -931,108 +875,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1052,6 +894,21 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1071,6 +928,18 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1090,6 +959,18 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1128,6 +1009,24 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1166,6 +1065,18 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1204,6 +1115,21 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1242,6 +1168,21 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1263,6 +1204,22 @@
     <dxf>
       <font>
         <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1309,6 +1266,117 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1407,8 +1475,8 @@
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="0" xr9:uid="{544401DC-1CE7-401F-8AEE-F889E0274DE0}"/>
     <tableStyle name="Table Style 2" pivot="0" count="2" xr9:uid="{067077C0-BF4C-48D1-B5BF-DFF53435431A}">
-      <tableStyleElement type="wholeTable" dxfId="100"/>
-      <tableStyleElement type="headerRow" dxfId="99"/>
+      <tableStyleElement type="wholeTable" dxfId="99"/>
+      <tableStyleElement type="headerRow" dxfId="98"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1423,67 +1491,67 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FA275680-42C1-4CF5-9E62-42189E8A54FD}" name="Table1" displayName="Table1" ref="B72:F81" totalsRowShown="0" headerRowDxfId="98" dataDxfId="97">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FA275680-42C1-4CF5-9E62-42189E8A54FD}" name="Table1" displayName="Table1" ref="B72:F81" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96">
   <autoFilter ref="B72:F81" xr:uid="{FA275680-42C1-4CF5-9E62-42189E8A54FD}"/>
   <tableColumns count="5">
-    <tableColumn id="2" xr3:uid="{983B3321-F8D6-4B25-9AC8-187F8F3D33CC}" name="Sr. No." dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{F86F5107-9EFE-4314-969C-E6DCD9A59B13}" name="Priority" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{7768FE33-8E07-4F5D-B874-306D7FC0ACB4}" name="Segment" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{AA766249-D3BA-403B-8A4B-9D3CB0E8DDF6}" name="Notes" dataDxfId="96"/>
-    <tableColumn id="6" xr3:uid="{DC096C63-8440-4369-AFCD-C38D5E75FDB4}" name="Status" dataDxfId="95"/>
+    <tableColumn id="2" xr3:uid="{983B3321-F8D6-4B25-9AC8-187F8F3D33CC}" name="Sr. No." dataDxfId="95"/>
+    <tableColumn id="3" xr3:uid="{F86F5107-9EFE-4314-969C-E6DCD9A59B13}" name="Priority" dataDxfId="94"/>
+    <tableColumn id="4" xr3:uid="{7768FE33-8E07-4F5D-B874-306D7FC0ACB4}" name="Segment" dataDxfId="93"/>
+    <tableColumn id="5" xr3:uid="{AA766249-D3BA-403B-8A4B-9D3CB0E8DDF6}" name="Notes" dataDxfId="92"/>
+    <tableColumn id="6" xr3:uid="{DC096C63-8440-4369-AFCD-C38D5E75FDB4}" name="Status" dataDxfId="91"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{2FCCE20B-9E13-410F-BE75-DE5F3889681F}" name="Table5101112" displayName="Table5101112" ref="B7:F18" totalsRowShown="0" headerRowDxfId="86">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{2FCCE20B-9E13-410F-BE75-DE5F3889681F}" name="Table5101112" displayName="Table5101112" ref="B7:F18" totalsRowShown="0" headerRowDxfId="44">
   <autoFilter ref="B7:F18" xr:uid="{2FCCE20B-9E13-410F-BE75-DE5F3889681F}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{C69E375F-3031-4D04-8599-C1718F971FB3}" name="Sr. No." dataDxfId="59"/>
-    <tableColumn id="2" xr3:uid="{19E69D82-0BA1-49A3-B646-3C0DC0440D74}" name="Subject Name" dataDxfId="60"/>
-    <tableColumn id="5" xr3:uid="{5ADEA569-AFEF-4F9E-A1E1-C44C8DB3092B}" name="Completion status" dataDxfId="63"/>
-    <tableColumn id="3" xr3:uid="{983EC962-947B-4AA7-9C4C-BDDB57A3875B}" name="Qs Done like ( ISI , CMI , PYQs)" dataDxfId="66"/>
-    <tableColumn id="4" xr3:uid="{69E8AE71-D2EA-4AF3-A141-699B1786925D}" name="Book referred" dataDxfId="68"/>
+    <tableColumn id="1" xr3:uid="{C69E375F-3031-4D04-8599-C1718F971FB3}" name="Sr. No." dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{19E69D82-0BA1-49A3-B646-3C0DC0440D74}" name="Subject Name" dataDxfId="42"/>
+    <tableColumn id="5" xr3:uid="{5ADEA569-AFEF-4F9E-A1E1-C44C8DB3092B}" name="Completion status" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{983EC962-947B-4AA7-9C4C-BDDB57A3875B}" name="Qs Done like ( ISI , CMI , PYQs)" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{69E8AE71-D2EA-4AF3-A141-699B1786925D}" name="Book referred" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{3821DA3F-058B-4D22-85EB-552E85DECF38}" name="Table510111213" displayName="Table510111213" ref="B23:F34" totalsRowShown="0" headerRowDxfId="85">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{3821DA3F-058B-4D22-85EB-552E85DECF38}" name="Table510111213" displayName="Table510111213" ref="B23:F34" totalsRowShown="0" headerRowDxfId="38">
   <autoFilter ref="B23:F34" xr:uid="{3821DA3F-058B-4D22-85EB-552E85DECF38}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{0E949512-5EFC-4406-90B5-209C463AB115}" name="Sr. No." dataDxfId="57"/>
-    <tableColumn id="6" xr3:uid="{8AA04A1B-943C-42A7-84BF-B1CC07DF59F1}" name="Score out of 100" dataDxfId="58"/>
-    <tableColumn id="2" xr3:uid="{2310352E-C67A-4717-B65B-0CBB557A1738}" name="Source" dataDxfId="62"/>
-    <tableColumn id="5" xr3:uid="{3C858A90-A9B9-430C-A005-36B4C374CE02}" name="Configuration" dataDxfId="65"/>
-    <tableColumn id="7" xr3:uid="{2EB8A9F3-05ED-48C6-89C2-FD3574C610B4}" name="Is unsolved are completed ?" dataDxfId="67"/>
+    <tableColumn id="1" xr3:uid="{0E949512-5EFC-4406-90B5-209C463AB115}" name="Sr. No." dataDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{8AA04A1B-943C-42A7-84BF-B1CC07DF59F1}" name="Score out of 100" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{2310352E-C67A-4717-B65B-0CBB557A1738}" name="Source" dataDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{3C858A90-A9B9-430C-A005-36B4C374CE02}" name="Configuration" dataDxfId="34"/>
+    <tableColumn id="7" xr3:uid="{2EB8A9F3-05ED-48C6-89C2-FD3574C610B4}" name="Is unsolved are completed ?" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{2950B954-0F8D-4547-B6D0-F8A1E3D44464}" name="Table51011121314" displayName="Table51011121314" ref="B39:E50" totalsRowShown="0" headerRowDxfId="84">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{2950B954-0F8D-4547-B6D0-F8A1E3D44464}" name="Table51011121314" displayName="Table51011121314" ref="B39:E50" totalsRowShown="0" headerRowDxfId="32">
   <autoFilter ref="B39:E50" xr:uid="{2950B954-0F8D-4547-B6D0-F8A1E3D44464}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{40F40B53-6367-431B-9A3C-0691502928F0}" name="Sr. No." dataDxfId="55"/>
-    <tableColumn id="6" xr3:uid="{BD38871E-72E7-4BD4-8FDD-3D44C72E5E47}" name="Subject" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{F2412BCA-894F-4900-919B-5611503549D0}" name="Source" dataDxfId="61"/>
-    <tableColumn id="5" xr3:uid="{102336CF-78DD-4991-BF27-5DCC2F63052C}" name="Configuration" dataDxfId="64"/>
+    <tableColumn id="1" xr3:uid="{40F40B53-6367-431B-9A3C-0691502928F0}" name="Sr. No." dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{BD38871E-72E7-4BD4-8FDD-3D44C72E5E47}" name="Subject" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{F2412BCA-894F-4900-919B-5611503549D0}" name="Source" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{102336CF-78DD-4991-BF27-5DCC2F63052C}" name="Configuration" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{96385616-5283-402C-B5CE-F5CA00597B81}" name="Table510111215" displayName="Table510111215" ref="B7:F18" totalsRowShown="0" headerRowDxfId="83">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{96385616-5283-402C-B5CE-F5CA00597B81}" name="Table510111215" displayName="Table510111215" ref="B7:F18" totalsRowShown="0" headerRowDxfId="27">
   <autoFilter ref="B7:F18" xr:uid="{96385616-5283-402C-B5CE-F5CA00597B81}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{1AA4D51E-6696-4F3B-819D-CED502D19759}" name="Sr. No." dataDxfId="77"/>
-    <tableColumn id="2" xr3:uid="{A5A3B651-A5AE-4567-9EBD-8A9988CC18E5}" name="Subject Name" dataDxfId="74"/>
-    <tableColumn id="5" xr3:uid="{5359417D-FD4D-4AD7-9751-4480B33E5853}" name="Completion status" dataDxfId="73"/>
+    <tableColumn id="1" xr3:uid="{1AA4D51E-6696-4F3B-819D-CED502D19759}" name="Sr. No." dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{A5A3B651-A5AE-4567-9EBD-8A9988CC18E5}" name="Subject Name" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{5359417D-FD4D-4AD7-9751-4480B33E5853}" name="Completion status" dataDxfId="24"/>
     <tableColumn id="3" xr3:uid="{2C72DCF7-BF48-4E1D-A2AB-2D555B056FBB}" name="Practice Qs Done of"/>
     <tableColumn id="4" xr3:uid="{77118590-8704-4795-8598-63CAF4812F03}" name="Book referred"/>
   </tableColumns>
@@ -1492,12 +1560,12 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{BA68BAC6-AE80-4845-94AE-7B887A62007A}" name="Table51011121316" displayName="Table51011121316" ref="B23:F34" totalsRowShown="0" headerRowDxfId="82">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{BA68BAC6-AE80-4845-94AE-7B887A62007A}" name="Table51011121316" displayName="Table51011121316" ref="B23:F34" totalsRowShown="0" headerRowDxfId="23">
   <autoFilter ref="B23:F34" xr:uid="{BA68BAC6-AE80-4845-94AE-7B887A62007A}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{FF6ACDE7-81AF-4834-B1D2-22B88FB52740}" name="Sr. No." dataDxfId="76"/>
-    <tableColumn id="6" xr3:uid="{F7B5120E-EE86-4DA2-9377-58F313198AAA}" name="Score out of 100" dataDxfId="72"/>
-    <tableColumn id="2" xr3:uid="{69495E51-BFF8-4D4A-8E14-76F93C0979E5}" name="Source" dataDxfId="71"/>
+    <tableColumn id="1" xr3:uid="{FF6ACDE7-81AF-4834-B1D2-22B88FB52740}" name="Sr. No." dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{F7B5120E-EE86-4DA2-9377-58F313198AAA}" name="Score out of 100" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{69495E51-BFF8-4D4A-8E14-76F93C0979E5}" name="Source" dataDxfId="20"/>
     <tableColumn id="5" xr3:uid="{EC2AC9E1-8CA1-4235-9B12-8F96F7AF5FBA}" name="Configuration"/>
     <tableColumn id="7" xr3:uid="{748FC77C-19E1-43C7-8297-634E2B7B6C19}" name="Is unsolved are completed ?"/>
   </tableColumns>
@@ -1506,12 +1574,12 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{6BD1E29E-6C21-4870-8FD3-724B9FBA07AC}" name="Table5101112131417" displayName="Table5101112131417" ref="B39:E50" totalsRowShown="0" headerRowDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{6BD1E29E-6C21-4870-8FD3-724B9FBA07AC}" name="Table5101112131417" displayName="Table5101112131417" ref="B39:E50" totalsRowShown="0" headerRowDxfId="19">
   <autoFilter ref="B39:E50" xr:uid="{6BD1E29E-6C21-4870-8FD3-724B9FBA07AC}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9012466F-3463-4516-BD4F-6CEF3F171ED9}" name="Sr. No." dataDxfId="75"/>
-    <tableColumn id="6" xr3:uid="{02F0E194-E997-4DA9-9CA7-D3FD99A17078}" name="Subject" dataDxfId="70"/>
-    <tableColumn id="2" xr3:uid="{63382DB5-C0ED-450D-A200-3D03099EAC8F}" name="Source" dataDxfId="69"/>
+    <tableColumn id="1" xr3:uid="{9012466F-3463-4516-BD4F-6CEF3F171ED9}" name="Sr. No." dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{02F0E194-E997-4DA9-9CA7-D3FD99A17078}" name="Subject" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{63382DB5-C0ED-450D-A200-3D03099EAC8F}" name="Source" dataDxfId="16"/>
     <tableColumn id="5" xr3:uid="{8FB0A8F1-B7E5-4C7D-97B9-A5E3621B0E0A}" name="Configuration"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1519,125 +1587,124 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{7F6A6026-7A1F-445F-BC12-0C62270D0992}" name="Table518" displayName="Table518" ref="A1:E9" totalsRowShown="0" headerRowDxfId="80">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{7F6A6026-7A1F-445F-BC12-0C62270D0992}" name="Table518" displayName="Table518" ref="A1:E9" totalsRowShown="0" headerRowDxfId="15">
   <autoFilter ref="A1:E9" xr:uid="{7F6A6026-7A1F-445F-BC12-0C62270D0992}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{20891DE8-4371-4821-9952-9906FE5FD3A0}" name="Semester" dataDxfId="79"/>
-    <tableColumn id="2" xr3:uid="{21267C3F-D1B9-4821-8C39-301BE85331F1}" name="Earned Credits ( grades * points )" dataDxfId="78"/>
-    <tableColumn id="3" xr3:uid="{C9CB8E24-F639-488B-9B6B-5D0B0534E7D4}" name="Total Credit Points" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{4BF2BE39-25EC-4855-8B2A-0AA4A4ACC357}" name="SGPA" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{15705279-D055-4C91-A1FB-C2318F8DB737}" name="CGPA" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{20891DE8-4371-4821-9952-9906FE5FD3A0}" name="Semester" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{21267C3F-D1B9-4821-8C39-301BE85331F1}" name="Earned Credits ( grades * points )" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{C9CB8E24-F639-488B-9B6B-5D0B0534E7D4}" name="Total Credit Points" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{4BF2BE39-25EC-4855-8B2A-0AA4A4ACC357}" name="SGPA" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{15705279-D055-4C91-A1FB-C2318F8DB737}" name="CGPA" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6875C3DB-155D-480E-87DC-9FFB83877AE4}" name="Table134" displayName="Table134" ref="C8:E22" totalsRowShown="0" headerRowDxfId="94">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6875C3DB-155D-480E-87DC-9FFB83877AE4}" name="Table134" displayName="Table134" ref="C8:E22" totalsRowShown="0" headerRowDxfId="90">
   <autoFilter ref="C8:E22" xr:uid="{6875C3DB-155D-480E-87DC-9FFB83877AE4}"/>
   <tableColumns count="3">
-    <tableColumn id="2" xr3:uid="{D58BACB9-C929-4657-A941-1C7BCD578EDF}" name="Sr. No." dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{2C6EBFA5-520C-473D-BBAC-0D5F31F4B191}" name="Segments" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{369550EE-78CE-4F66-875F-F34D301E4A0E}" name="Status" dataDxfId="93"/>
+    <tableColumn id="2" xr3:uid="{D58BACB9-C929-4657-A941-1C7BCD578EDF}" name="Sr. No." dataDxfId="89"/>
+    <tableColumn id="3" xr3:uid="{2C6EBFA5-520C-473D-BBAC-0D5F31F4B191}" name="Segments" dataDxfId="88"/>
+    <tableColumn id="6" xr3:uid="{369550EE-78CE-4F66-875F-F34D301E4A0E}" name="Status" dataDxfId="87"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{788F11B4-6638-437A-BA2F-755567F822A6}" name="Table1345" displayName="Table1345" ref="C27:E67" totalsRowShown="0" headerRowDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{788F11B4-6638-437A-BA2F-755567F822A6}" name="Table1345" displayName="Table1345" ref="C27:E67" totalsRowShown="0" headerRowDxfId="86">
   <autoFilter ref="C27:E67" xr:uid="{788F11B4-6638-437A-BA2F-755567F822A6}"/>
   <tableColumns count="3">
-    <tableColumn id="5" xr3:uid="{760912DC-252C-490D-ABB6-BB7CFB907BE3}" name="Sr. No." dataDxfId="12"/>
-    <tableColumn id="1" xr3:uid="{7CB8FDA8-DE34-41AD-A040-9BC8A65E7DD5}" name="Segment" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{528137CC-3CA7-445D-8720-7662B0C9A622}" name="Status" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{760912DC-252C-490D-ABB6-BB7CFB907BE3}" name="Sr. No." dataDxfId="85"/>
+    <tableColumn id="1" xr3:uid="{7CB8FDA8-DE34-41AD-A040-9BC8A65E7DD5}" name="Segment" dataDxfId="84"/>
+    <tableColumn id="6" xr3:uid="{528137CC-3CA7-445D-8720-7662B0C9A622}" name="Status" dataDxfId="83"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{84452A60-847A-4B8A-83CA-A4FCDAA63125}" name="Table5" displayName="Table5" ref="A4:F15" totalsRowShown="0" headerRowDxfId="92">
-  <autoFilter ref="A4:F15" xr:uid="{84452A60-847A-4B8A-83CA-A4FCDAA63125}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{84452A60-847A-4B8A-83CA-A4FCDAA63125}" name="Table5" displayName="Table5" ref="A4:F16" totalsRowShown="0" headerRowDxfId="82">
+  <autoFilter ref="A4:F16" xr:uid="{84452A60-847A-4B8A-83CA-A4FCDAA63125}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{098856E3-B02E-485D-9D0F-E29E193105C2}" name="Sr. No." dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{83B343C4-EFBE-4603-8040-574FF38A5C51}" name="Problem Number" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{AE24D3A9-D4C4-46A6-99F5-433AE03DAEF9}" name="Problem Name " dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{9920FB77-EF34-497B-93AE-9F7763415894}" name="Topics" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{D1A3124C-004E-45D4-954E-AA76640B7937}" name="No. of submissions" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{56B65B9A-310D-4041-89C7-B0A8CED57837}" name="Approach" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{098856E3-B02E-485D-9D0F-E29E193105C2}" name="Sr. No." dataDxfId="81"/>
+    <tableColumn id="2" xr3:uid="{83B343C4-EFBE-4603-8040-574FF38A5C51}" name="Problem No." dataDxfId="80"/>
+    <tableColumn id="3" xr3:uid="{AE24D3A9-D4C4-46A6-99F5-433AE03DAEF9}" name="Problem Name " dataDxfId="79"/>
+    <tableColumn id="4" xr3:uid="{9920FB77-EF34-497B-93AE-9F7763415894}" name="Topics" dataDxfId="78"/>
+    <tableColumn id="5" xr3:uid="{D1A3124C-004E-45D4-954E-AA76640B7937}" name="# successful submissions" dataDxfId="77"/>
+    <tableColumn id="6" xr3:uid="{56B65B9A-310D-4041-89C7-B0A8CED57837}" name="Approach" dataDxfId="76"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{5BC27E0C-9DF6-4031-8FA8-7A854E192CF8}" name="Table57" displayName="Table57" ref="A4:F15" totalsRowShown="0" headerRowDxfId="91">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{5BC27E0C-9DF6-4031-8FA8-7A854E192CF8}" name="Table57" displayName="Table57" ref="A4:F15" totalsRowShown="0" headerRowDxfId="75">
   <autoFilter ref="A4:F15" xr:uid="{5BC27E0C-9DF6-4031-8FA8-7A854E192CF8}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{9651C52B-7806-43A6-91F8-B23AA14F41C3}" name="Sr. No." dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{3A9713D4-F647-485B-A4A0-2715CB1510EB}" name="Problem Number" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{7A0FF35D-6B52-4F27-99C5-2F48786B9CE3}" name="Problem Name " dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{B7E260E6-D6FA-43B8-B1D9-56E22620F278}" name="Topics" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{440BA5E6-E0EA-4BE8-ACF8-216A362EF353}" name="No. of submissions" dataDxfId="28"/>
-    <tableColumn id="6" xr3:uid="{CB6EB9E7-10CE-455D-898A-DD7B9E8F7336}" name="Approach" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{9651C52B-7806-43A6-91F8-B23AA14F41C3}" name="Sr. No." dataDxfId="74"/>
+    <tableColumn id="2" xr3:uid="{3A9713D4-F647-485B-A4A0-2715CB1510EB}" name="Problem Number" dataDxfId="73"/>
+    <tableColumn id="3" xr3:uid="{7A0FF35D-6B52-4F27-99C5-2F48786B9CE3}" name="Problem Name " dataDxfId="72"/>
+    <tableColumn id="4" xr3:uid="{B7E260E6-D6FA-43B8-B1D9-56E22620F278}" name="Topics" dataDxfId="71"/>
+    <tableColumn id="5" xr3:uid="{440BA5E6-E0EA-4BE8-ACF8-216A362EF353}" name="No. of submissions" dataDxfId="70"/>
+    <tableColumn id="6" xr3:uid="{CB6EB9E7-10CE-455D-898A-DD7B9E8F7336}" name="Approach" dataDxfId="69"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9E1DEB40-0F05-4D65-9FB8-B45BE5A82EF6}" name="Table578" displayName="Table578" ref="A4:F15" totalsRowShown="0" headerRowDxfId="90">
-  <autoFilter ref="A4:F15" xr:uid="{9E1DEB40-0F05-4D65-9FB8-B45BE5A82EF6}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{6A952779-BA13-46EA-9B96-3D7A0BC96174}" name="Sr. No." dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{14AF1FFB-7EDD-45A3-BB3F-75B548639663}" name="Problem Number" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{E09E5E6F-9F1D-4ABD-9DB0-2790C6978460}" name="Problem Name " dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{6D8B390F-6B02-4BF2-99E8-2302EC294D13}" name="Topics" dataDxfId="36"/>
-    <tableColumn id="5" xr3:uid="{CD7B5BF8-E6ED-4B3D-8CE7-57CEBE20D38B}" name="No. of submissions" dataDxfId="35"/>
-    <tableColumn id="6" xr3:uid="{BB289159-FCF4-49E7-9D05-2942567C89DB}" name="Approach" dataDxfId="34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9E1DEB40-0F05-4D65-9FB8-B45BE5A82EF6}" name="Table578" displayName="Table578" ref="A4:E15" totalsRowShown="0" headerRowDxfId="68">
+  <autoFilter ref="A4:E15" xr:uid="{9E1DEB40-0F05-4D65-9FB8-B45BE5A82EF6}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{6A952779-BA13-46EA-9B96-3D7A0BC96174}" name="Sr. No." dataDxfId="67"/>
+    <tableColumn id="3" xr3:uid="{E09E5E6F-9F1D-4ABD-9DB0-2790C6978460}" name="Problem Name " dataDxfId="66"/>
+    <tableColumn id="4" xr3:uid="{6D8B390F-6B02-4BF2-99E8-2302EC294D13}" name="Topics" dataDxfId="65"/>
+    <tableColumn id="5" xr3:uid="{CD7B5BF8-E6ED-4B3D-8CE7-57CEBE20D38B}" name="No. of submissions" dataDxfId="64"/>
+    <tableColumn id="6" xr3:uid="{BB289159-FCF4-49E7-9D05-2942567C89DB}" name="Approach" dataDxfId="63"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{672760BD-9E09-4244-BF94-EBE4882DE481}" name="Table5789" displayName="Table5789" ref="A4:G15" totalsRowShown="0" headerRowDxfId="89">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{672760BD-9E09-4244-BF94-EBE4882DE481}" name="Table5789" displayName="Table5789" ref="A4:G15" totalsRowShown="0" headerRowDxfId="62">
   <autoFilter ref="A4:G15" xr:uid="{672760BD-9E09-4244-BF94-EBE4882DE481}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{7FC01D48-50FB-4B71-85D4-13D6B6A8B170}" name="Sr. No." dataDxfId="46"/>
-    <tableColumn id="2" xr3:uid="{F5B46941-4EA0-413A-B16F-998B34562FA9}" name="Platform name" dataDxfId="45"/>
-    <tableColumn id="3" xr3:uid="{11183BC0-200E-4A30-B5B7-5AD6ED263B71}" name="Contest Details" dataDxfId="44"/>
-    <tableColumn id="4" xr3:uid="{E99F4D16-1AFB-4115-A8C2-92F4F12E75F0}" name="# total Qs" dataDxfId="43"/>
-    <tableColumn id="7" xr3:uid="{D4124943-F8BF-4815-B6B9-91C683C8A94C}" name="# Solved Qs" dataDxfId="42"/>
-    <tableColumn id="5" xr3:uid="{6A1CC701-3B3F-48D6-A63E-0D0D28D38855}" name="Ranking" dataDxfId="41"/>
-    <tableColumn id="6" xr3:uid="{2DF92217-CA09-48F3-B4F6-01C752A7709A}" name="Are remainings solved ?" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{7FC01D48-50FB-4B71-85D4-13D6B6A8B170}" name="Sr. No." dataDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{F5B46941-4EA0-413A-B16F-998B34562FA9}" name="Platform name" dataDxfId="60"/>
+    <tableColumn id="3" xr3:uid="{11183BC0-200E-4A30-B5B7-5AD6ED263B71}" name="Contest Details" dataDxfId="59"/>
+    <tableColumn id="4" xr3:uid="{E99F4D16-1AFB-4115-A8C2-92F4F12E75F0}" name="# total Qs" dataDxfId="58"/>
+    <tableColumn id="7" xr3:uid="{D4124943-F8BF-4815-B6B9-91C683C8A94C}" name="# Solved Qs" dataDxfId="57"/>
+    <tableColumn id="5" xr3:uid="{6A1CC701-3B3F-48D6-A63E-0D0D28D38855}" name="Ranking" dataDxfId="56"/>
+    <tableColumn id="6" xr3:uid="{2DF92217-CA09-48F3-B4F6-01C752A7709A}" name="Are remainings solved ?" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{C7ACFC98-5037-44D8-82A3-B31E6683EF89}" name="Table510" displayName="Table510" ref="C4:F15" totalsRowShown="0" headerRowDxfId="88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{C7ACFC98-5037-44D8-82A3-B31E6683EF89}" name="Table510" displayName="Table510" ref="C4:F15" totalsRowShown="0" headerRowDxfId="54">
   <autoFilter ref="C4:F15" xr:uid="{C7ACFC98-5037-44D8-82A3-B31E6683EF89}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{38FEAE95-18E2-4FE0-BD6A-9BE906D4AFCC}" name="Sr. No." dataDxfId="50"/>
-    <tableColumn id="2" xr3:uid="{515E0F35-8C77-4BD4-99B5-16D2F593FC0D}" name="Project name" dataDxfId="49"/>
-    <tableColumn id="3" xr3:uid="{ED1A562C-F12C-46A6-A207-873D0289DC8F}" name="Skills used " dataDxfId="48"/>
-    <tableColumn id="4" xr3:uid="{484475D7-C606-4DEC-88C4-3D78EDF74E20}" name="Notes about it" dataDxfId="47"/>
+    <tableColumn id="1" xr3:uid="{38FEAE95-18E2-4FE0-BD6A-9BE906D4AFCC}" name="Sr. No." dataDxfId="53"/>
+    <tableColumn id="2" xr3:uid="{515E0F35-8C77-4BD4-99B5-16D2F593FC0D}" name="Project name" dataDxfId="52"/>
+    <tableColumn id="3" xr3:uid="{ED1A562C-F12C-46A6-A207-873D0289DC8F}" name="Skills used " dataDxfId="51"/>
+    <tableColumn id="4" xr3:uid="{484475D7-C606-4DEC-88C4-3D78EDF74E20}" name="Notes about it" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{F04800D1-1296-49C2-9C89-FF4D36C3C5FA}" name="Table51011" displayName="Table51011" ref="C4:F15" totalsRowShown="0" headerRowDxfId="87">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{F04800D1-1296-49C2-9C89-FF4D36C3C5FA}" name="Table51011" displayName="Table51011" ref="C4:F15" totalsRowShown="0" headerRowDxfId="49">
   <autoFilter ref="C4:F15" xr:uid="{F04800D1-1296-49C2-9C89-FF4D36C3C5FA}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{75C622E8-8C93-498B-BB53-4AB82294F580}" name="Sr. No." dataDxfId="54"/>
-    <tableColumn id="2" xr3:uid="{491A9B10-7CCF-4151-BC22-1F881029D1CF}" name="Book name" dataDxfId="53"/>
-    <tableColumn id="3" xr3:uid="{79454B67-6983-4C7D-8F1A-1ABD4C8AA5EB}" name="Author " dataDxfId="52"/>
-    <tableColumn id="4" xr3:uid="{9F631DF3-35C9-4F10-AAF7-8FC855753250}" name="Learnings" dataDxfId="51"/>
+    <tableColumn id="1" xr3:uid="{75C622E8-8C93-498B-BB53-4AB82294F580}" name="Sr. No." dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{491A9B10-7CCF-4151-BC22-1F881029D1CF}" name="Book name" dataDxfId="47"/>
+    <tableColumn id="3" xr3:uid="{79454B67-6983-4C7D-8F1A-1ABD4C8AA5EB}" name="Author " dataDxfId="46"/>
+    <tableColumn id="4" xr3:uid="{9F631DF3-35C9-4F10-AAF7-8FC855753250}" name="Learnings" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1942,8 +2009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA808F5-CFD7-47C2-A961-FADC6CC1CBFE}">
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView showGridLines="0" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="G75" sqref="G75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1957,52 +2024,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
     </row>
     <row r="2" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
     </row>
     <row r="3" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
     </row>
     <row r="6" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
     </row>
     <row r="7" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
     </row>
     <row r="8" spans="1:8" s="6" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="7"/>
@@ -2010,7 +2077,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>14</v>
@@ -2021,7 +2088,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>25</v>
@@ -2033,7 +2100,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>25</v>
@@ -2045,7 +2112,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>25</v>
@@ -2057,7 +2124,7 @@
         <v>4</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>25</v>
@@ -2069,7 +2136,7 @@
         <v>5</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>25</v>
@@ -2081,7 +2148,7 @@
         <v>6</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>25</v>
@@ -2093,7 +2160,7 @@
         <v>7</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>25</v>
@@ -2105,7 +2172,7 @@
         <v>8</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>25</v>
@@ -2117,7 +2184,7 @@
         <v>9</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>25</v>
@@ -2129,7 +2196,7 @@
         <v>10</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>25</v>
@@ -2141,7 +2208,7 @@
         <v>11</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>25</v>
@@ -2153,7 +2220,7 @@
         <v>12</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>25</v>
@@ -2165,7 +2232,7 @@
         <v>13</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>25</v>
@@ -2174,35 +2241,35 @@
     </row>
     <row r="22" spans="2:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C22" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F22"/>
     </row>
     <row r="25" spans="2:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
     </row>
     <row r="26" spans="2:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
     </row>
     <row r="27" spans="2:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C27" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>14</v>
@@ -2214,7 +2281,7 @@
         <v>1</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>25</v>
@@ -2226,7 +2293,7 @@
         <v>2</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>25</v>
@@ -2238,7 +2305,7 @@
         <v>4</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>25</v>
@@ -2250,7 +2317,7 @@
         <v>5</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>25</v>
@@ -2262,7 +2329,7 @@
         <v>6</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>25</v>
@@ -2274,7 +2341,7 @@
         <v>7</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>25</v>
@@ -2286,7 +2353,7 @@
         <v>8</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>25</v>
@@ -2298,7 +2365,7 @@
         <v>9</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>25</v>
@@ -2310,7 +2377,7 @@
         <v>10</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>25</v>
@@ -2322,7 +2389,7 @@
         <v>11</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>25</v>
@@ -2334,7 +2401,7 @@
         <v>12</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>25</v>
@@ -2346,7 +2413,7 @@
         <v>13</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>25</v>
@@ -2358,7 +2425,7 @@
         <v>14</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>25</v>
@@ -2370,7 +2437,7 @@
         <v>15</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>25</v>
@@ -2385,7 +2452,7 @@
         <v>16</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>25</v>
@@ -2397,7 +2464,7 @@
         <v>17</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>25</v>
@@ -2409,7 +2476,7 @@
         <v>18</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>25</v>
@@ -2421,7 +2488,7 @@
         <v>19</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>25</v>
@@ -2433,7 +2500,7 @@
         <v>20</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>25</v>
@@ -2445,7 +2512,7 @@
         <v>21</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>25</v>
@@ -2457,7 +2524,7 @@
         <v>22</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>25</v>
@@ -2469,7 +2536,7 @@
         <v>23</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>25</v>
@@ -2481,7 +2548,7 @@
         <v>24</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>25</v>
@@ -2493,7 +2560,7 @@
         <v>25</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>25</v>
@@ -2505,7 +2572,7 @@
         <v>26</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>25</v>
@@ -2517,7 +2584,7 @@
         <v>27</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>25</v>
@@ -2529,7 +2596,7 @@
         <v>28</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>25</v>
@@ -2541,7 +2608,7 @@
         <v>29</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>25</v>
@@ -2553,7 +2620,7 @@
         <v>30</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>25</v>
@@ -2565,7 +2632,7 @@
         <v>31</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>25</v>
@@ -2577,7 +2644,7 @@
         <v>32</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>25</v>
@@ -2589,7 +2656,7 @@
         <v>33</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>25</v>
@@ -2601,7 +2668,7 @@
         <v>34</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>25</v>
@@ -2613,7 +2680,7 @@
         <v>35</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>25</v>
@@ -2625,7 +2692,7 @@
         <v>36</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>25</v>
@@ -2640,7 +2707,7 @@
         <v>37</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>25</v>
@@ -2652,7 +2719,7 @@
         <v>38</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>25</v>
@@ -2663,20 +2730,20 @@
       <c r="F67"/>
     </row>
     <row r="70" spans="2:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="8" t="s">
+      <c r="B70" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C70" s="8"/>
-      <c r="D70" s="8"/>
-      <c r="E70" s="8"/>
-      <c r="F70" s="8"/>
+      <c r="C70" s="10"/>
+      <c r="D70" s="10"/>
+      <c r="E70" s="10"/>
+      <c r="F70" s="10"/>
     </row>
     <row r="71" spans="2:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="8"/>
-      <c r="C71" s="8"/>
-      <c r="D71" s="8"/>
-      <c r="E71" s="8"/>
-      <c r="F71" s="8"/>
+      <c r="B71" s="10"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="10"/>
+      <c r="E71" s="10"/>
+      <c r="F71" s="10"/>
     </row>
     <row r="72" spans="2:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B72" s="7" t="s">
@@ -2685,8 +2752,8 @@
       <c r="C72" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D72" s="14" t="s">
-        <v>71</v>
+      <c r="D72" s="9" t="s">
+        <v>70</v>
       </c>
       <c r="E72" s="7" t="s">
         <v>20</v>
@@ -2702,8 +2769,8 @@
       <c r="C73" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D73" s="14" t="s">
-        <v>73</v>
+      <c r="D73" s="9" t="s">
+        <v>72</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>25</v>
@@ -2716,8 +2783,8 @@
       <c r="C74" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D74" s="14" t="s">
-        <v>74</v>
+      <c r="D74" s="9" t="s">
+        <v>73</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>25</v>
@@ -2730,8 +2797,8 @@
       <c r="C75" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D75" s="14" t="s">
-        <v>75</v>
+      <c r="D75" s="9" t="s">
+        <v>112</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>25</v>
@@ -2744,8 +2811,8 @@
       <c r="C76" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D76" s="14" t="s">
-        <v>72</v>
+      <c r="D76" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>25</v>
@@ -2758,11 +2825,11 @@
       <c r="C77" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D77" s="14" t="s">
-        <v>76</v>
+      <c r="D77" s="9" t="s">
+        <v>74</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>25</v>
+        <v>111</v>
       </c>
     </row>
     <row r="78" spans="2:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -2772,27 +2839,27 @@
       <c r="C78" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D78" s="14" t="s">
-        <v>77</v>
+      <c r="D78" s="9" t="s">
+        <v>75</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="79" spans="2:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D79" s="14"/>
+      <c r="D79" s="9"/>
       <c r="F79" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="80" spans="2:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D80" s="14"/>
+      <c r="D80" s="9"/>
       <c r="F80" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="81" spans="4:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D81" s="14"/>
+      <c r="D81" s="9"/>
       <c r="F81" s="2" t="s">
         <v>25</v>
       </c>
@@ -2881,14 +2948,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>11</v>
@@ -2959,46 +3026,46 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{302BD800-2B4A-4BB0-AA56-AC69D49181F9}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="32" style="1" customWidth="1"/>
-    <col min="4" max="4" width="29.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="51.21875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.77734375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="30.77734375" style="1" customWidth="1"/>
     <col min="6" max="6" width="61.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:15" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="4" spans="1:15" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>2</v>
@@ -3007,17 +3074,66 @@
         <v>3</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>4</v>
+        <v>126</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" s="16" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="15">
+        <v>1</v>
+      </c>
+      <c r="B5" s="15">
+        <v>1</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="F5" s="2"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
+    <row r="6" spans="1:15" s="16" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="15">
+        <v>2</v>
+      </c>
+      <c r="B6" s="15">
+        <v>7</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
     <row r="7" spans="1:15" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="15">
+        <v>3</v>
+      </c>
+      <c r="B7" s="15">
+        <v>9</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>129</v>
+      </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -3025,6 +3141,103 @@
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
+    </row>
+    <row r="8" spans="1:15" s="16" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="15">
+        <v>4</v>
+      </c>
+      <c r="B8" s="15">
+        <v>26</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:15" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="15">
+        <v>5</v>
+      </c>
+      <c r="B9" s="15">
+        <v>1009</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" s="16" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="15">
+        <v>6</v>
+      </c>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:15" s="16" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="15">
+        <v>7</v>
+      </c>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:15" s="16" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="15">
+        <v>8</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:15" s="16" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:15" s="16" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:15" s="16" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:15" s="16" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3051,28 +3264,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -3140,87 +3353,182 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.77734375" defaultRowHeight="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="25.77734375" style="1"/>
+    <col min="1" max="1" width="17.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="46.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="34.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.77734375" style="1"/>
+    <col min="5" max="5" width="21.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="25.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="A1" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4"/>
+    </row>
+    <row r="5" spans="1:6" s="16" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="15">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="B5" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="15">
         <v>2</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" s="16" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="15">
+        <v>2</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="15">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" s="16" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="15">
         <v>3</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="B7" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" s="15">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" s="16" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="15">
         <v>4</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="B8" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" s="15">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" s="16" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="15">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F15" s="2"/>
+      <c r="B9" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="D9" s="15">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" s="16" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="15">
+        <v>6</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10" s="15">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" s="16" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" s="16" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" s="16" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" s="16" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" s="16" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3252,49 +3560,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
+      <c r="A1" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H4" s="5"/>
     </row>
@@ -3359,42 +3667,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
+      <c r="A1" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
     </row>
     <row r="2" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
     </row>
     <row r="3" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -3425,42 +3733,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
     </row>
     <row r="2" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
     </row>
     <row r="3" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -3493,142 +3801,142 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
     </row>
     <row r="2" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
     </row>
     <row r="3" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
+      <c r="A4" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
+      <c r="A20" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
     </row>
     <row r="21" spans="1:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
     </row>
     <row r="23" spans="1:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="4"/>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="13" t="s">
-        <v>46</v>
+      <c r="C23" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="36" spans="1:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
+      <c r="A36" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
     </row>
     <row r="37" spans="1:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
+      <c r="A37" s="14"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
     </row>
     <row r="39" spans="1:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="13" t="s">
+      <c r="B39" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -3667,142 +3975,142 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
     </row>
     <row r="2" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
     </row>
     <row r="3" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
+      <c r="A4" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
+      <c r="A20" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
     </row>
     <row r="21" spans="1:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
     </row>
     <row r="23" spans="1:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="4"/>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="13" t="s">
-        <v>46</v>
+      <c r="C23" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="36" spans="1:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
+      <c r="A36" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
     </row>
     <row r="37" spans="1:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
+      <c r="A37" s="14"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
     </row>
     <row r="39" spans="1:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="13" t="s">
+      <c r="B39" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updating the master sheet
</commit_message>
<xml_diff>
--- a/Master-Sheet.xlsx
+++ b/Master-Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OTHERS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC392BE-7A40-43B9-A165-BCBDB3CE67FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02840585-E7F0-44E6-9B35-F5F4A56B496F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="702" activeTab="6" xr2:uid="{0042A21B-FF33-4EBF-B65C-49274797135A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="702" activeTab="2" xr2:uid="{0042A21B-FF33-4EBF-B65C-49274797135A}"/>
   </bookViews>
   <sheets>
     <sheet name="LEETCODE " sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="139">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -424,6 +424,33 @@
   </si>
   <si>
     <t>Basic</t>
+  </si>
+  <si>
+    <t>Rotate Array</t>
+  </si>
+  <si>
+    <t>Peak Element</t>
+  </si>
+  <si>
+    <t>Binary Search</t>
+  </si>
+  <si>
+    <t>Equilibrium Point</t>
+  </si>
+  <si>
+    <t>Array Leaders</t>
+  </si>
+  <si>
+    <t>1 // 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1 // 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 // 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 // 7 </t>
   </si>
 </sst>
 </file>
@@ -608,16 +635,16 @@
     <xf numFmtId="16" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -922,15 +949,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -953,6 +984,208 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -984,6 +1217,18 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1003,24 +1248,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1040,6 +1267,24 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1059,18 +1304,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1090,6 +1323,18 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1109,21 +1354,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1143,6 +1373,21 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1162,21 +1407,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1196,19 +1426,18 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1229,208 +1458,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -1485,15 +1512,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{84452A60-847A-4B8A-83CA-A4FCDAA63125}" name="Table5" displayName="Table5" ref="A4:F16" totalsRowShown="0" headerRowDxfId="82">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{84452A60-847A-4B8A-83CA-A4FCDAA63125}" name="Table5" displayName="Table5" ref="A4:F16" totalsRowShown="0" headerRowDxfId="97">
   <autoFilter ref="A4:F16" xr:uid="{84452A60-847A-4B8A-83CA-A4FCDAA63125}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{098856E3-B02E-485D-9D0F-E29E193105C2}" name="Sr. No." dataDxfId="81"/>
-    <tableColumn id="2" xr3:uid="{83B343C4-EFBE-4603-8040-574FF38A5C51}" name="Problem No." dataDxfId="80"/>
-    <tableColumn id="3" xr3:uid="{AE24D3A9-D4C4-46A6-99F5-433AE03DAEF9}" name="Problem Name " dataDxfId="79"/>
-    <tableColumn id="4" xr3:uid="{9920FB77-EF34-497B-93AE-9F7763415894}" name="Topics" dataDxfId="78"/>
-    <tableColumn id="5" xr3:uid="{D1A3124C-004E-45D4-954E-AA76640B7937}" name="# successful submissions" dataDxfId="77"/>
-    <tableColumn id="6" xr3:uid="{56B65B9A-310D-4041-89C7-B0A8CED57837}" name="Approach" dataDxfId="76"/>
+    <tableColumn id="1" xr3:uid="{098856E3-B02E-485D-9D0F-E29E193105C2}" name="Sr. No." dataDxfId="96"/>
+    <tableColumn id="2" xr3:uid="{83B343C4-EFBE-4603-8040-574FF38A5C51}" name="Problem No." dataDxfId="95"/>
+    <tableColumn id="3" xr3:uid="{AE24D3A9-D4C4-46A6-99F5-433AE03DAEF9}" name="Problem Name " dataDxfId="94"/>
+    <tableColumn id="4" xr3:uid="{9920FB77-EF34-497B-93AE-9F7763415894}" name="Topics" dataDxfId="93"/>
+    <tableColumn id="5" xr3:uid="{D1A3124C-004E-45D4-954E-AA76640B7937}" name="# successful submissions" dataDxfId="92"/>
+    <tableColumn id="6" xr3:uid="{56B65B9A-310D-4041-89C7-B0A8CED57837}" name="Approach" dataDxfId="91"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1596,109 +1623,109 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{5BC27E0C-9DF6-4031-8FA8-7A854E192CF8}" name="Table57" displayName="Table57" ref="A4:F15" totalsRowShown="0" headerRowDxfId="75">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{5BC27E0C-9DF6-4031-8FA8-7A854E192CF8}" name="Table57" displayName="Table57" ref="A4:F15" totalsRowShown="0" headerRowDxfId="90">
   <autoFilter ref="A4:F15" xr:uid="{5BC27E0C-9DF6-4031-8FA8-7A854E192CF8}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{9651C52B-7806-43A6-91F8-B23AA14F41C3}" name="Sr. No." dataDxfId="74"/>
-    <tableColumn id="2" xr3:uid="{3A9713D4-F647-485B-A4A0-2715CB1510EB}" name="Problem Number" dataDxfId="73"/>
-    <tableColumn id="3" xr3:uid="{7A0FF35D-6B52-4F27-99C5-2F48786B9CE3}" name="Problem Name " dataDxfId="72"/>
-    <tableColumn id="4" xr3:uid="{B7E260E6-D6FA-43B8-B1D9-56E22620F278}" name="Topics" dataDxfId="71"/>
-    <tableColumn id="5" xr3:uid="{440BA5E6-E0EA-4BE8-ACF8-216A362EF353}" name="No. of submissions" dataDxfId="70"/>
-    <tableColumn id="6" xr3:uid="{CB6EB9E7-10CE-455D-898A-DD7B9E8F7336}" name="Approach" dataDxfId="69"/>
+    <tableColumn id="1" xr3:uid="{9651C52B-7806-43A6-91F8-B23AA14F41C3}" name="Sr. No." dataDxfId="89"/>
+    <tableColumn id="2" xr3:uid="{3A9713D4-F647-485B-A4A0-2715CB1510EB}" name="Problem Number" dataDxfId="88"/>
+    <tableColumn id="3" xr3:uid="{7A0FF35D-6B52-4F27-99C5-2F48786B9CE3}" name="Problem Name " dataDxfId="87"/>
+    <tableColumn id="4" xr3:uid="{B7E260E6-D6FA-43B8-B1D9-56E22620F278}" name="Topics" dataDxfId="86"/>
+    <tableColumn id="5" xr3:uid="{440BA5E6-E0EA-4BE8-ACF8-216A362EF353}" name="No. of submissions" dataDxfId="85"/>
+    <tableColumn id="6" xr3:uid="{CB6EB9E7-10CE-455D-898A-DD7B9E8F7336}" name="Approach" dataDxfId="84"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9E1DEB40-0F05-4D65-9FB8-B45BE5A82EF6}" name="Table578" displayName="Table578" ref="A4:E15" totalsRowShown="0" headerRowDxfId="68">
-  <autoFilter ref="A4:E15" xr:uid="{9E1DEB40-0F05-4D65-9FB8-B45BE5A82EF6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9E1DEB40-0F05-4D65-9FB8-B45BE5A82EF6}" name="Table578" displayName="Table578" ref="A4:E17" totalsRowShown="0" headerRowDxfId="83">
+  <autoFilter ref="A4:E17" xr:uid="{9E1DEB40-0F05-4D65-9FB8-B45BE5A82EF6}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{6A952779-BA13-46EA-9B96-3D7A0BC96174}" name="Sr. No." dataDxfId="67"/>
-    <tableColumn id="3" xr3:uid="{E09E5E6F-9F1D-4ABD-9DB0-2790C6978460}" name="Problem Name " dataDxfId="66"/>
-    <tableColumn id="4" xr3:uid="{6D8B390F-6B02-4BF2-99E8-2302EC294D13}" name="Topics" dataDxfId="65"/>
-    <tableColumn id="5" xr3:uid="{CD7B5BF8-E6ED-4B3D-8CE7-57CEBE20D38B}" name="No. of submissions" dataDxfId="64"/>
-    <tableColumn id="6" xr3:uid="{BB289159-FCF4-49E7-9D05-2942567C89DB}" name="Approach" dataDxfId="63"/>
+    <tableColumn id="1" xr3:uid="{6A952779-BA13-46EA-9B96-3D7A0BC96174}" name="Sr. No." dataDxfId="82"/>
+    <tableColumn id="3" xr3:uid="{E09E5E6F-9F1D-4ABD-9DB0-2790C6978460}" name="Problem Name " dataDxfId="81"/>
+    <tableColumn id="4" xr3:uid="{6D8B390F-6B02-4BF2-99E8-2302EC294D13}" name="Topics" dataDxfId="80"/>
+    <tableColumn id="5" xr3:uid="{CD7B5BF8-E6ED-4B3D-8CE7-57CEBE20D38B}" name="No. of submissions" dataDxfId="79"/>
+    <tableColumn id="6" xr3:uid="{BB289159-FCF4-49E7-9D05-2942567C89DB}" name="Approach" dataDxfId="78"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{672760BD-9E09-4244-BF94-EBE4882DE481}" name="Table5789" displayName="Table5789" ref="A4:G15" totalsRowShown="0" headerRowDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{672760BD-9E09-4244-BF94-EBE4882DE481}" name="Table5789" displayName="Table5789" ref="A4:G15" totalsRowShown="0" headerRowDxfId="77">
   <autoFilter ref="A4:G15" xr:uid="{672760BD-9E09-4244-BF94-EBE4882DE481}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{7FC01D48-50FB-4B71-85D4-13D6B6A8B170}" name="Sr. No." dataDxfId="61"/>
-    <tableColumn id="2" xr3:uid="{F5B46941-4EA0-413A-B16F-998B34562FA9}" name="Platform name" dataDxfId="60"/>
-    <tableColumn id="3" xr3:uid="{11183BC0-200E-4A30-B5B7-5AD6ED263B71}" name="Contest Details" dataDxfId="59"/>
-    <tableColumn id="4" xr3:uid="{E99F4D16-1AFB-4115-A8C2-92F4F12E75F0}" name="# total Qs" dataDxfId="58"/>
-    <tableColumn id="7" xr3:uid="{D4124943-F8BF-4815-B6B9-91C683C8A94C}" name="# Solved Qs" dataDxfId="57"/>
-    <tableColumn id="5" xr3:uid="{6A1CC701-3B3F-48D6-A63E-0D0D28D38855}" name="Ranking" dataDxfId="56"/>
-    <tableColumn id="6" xr3:uid="{2DF92217-CA09-48F3-B4F6-01C752A7709A}" name="Are remainings solved ?" dataDxfId="55"/>
+    <tableColumn id="1" xr3:uid="{7FC01D48-50FB-4B71-85D4-13D6B6A8B170}" name="Sr. No." dataDxfId="76"/>
+    <tableColumn id="2" xr3:uid="{F5B46941-4EA0-413A-B16F-998B34562FA9}" name="Platform name" dataDxfId="75"/>
+    <tableColumn id="3" xr3:uid="{11183BC0-200E-4A30-B5B7-5AD6ED263B71}" name="Contest Details" dataDxfId="74"/>
+    <tableColumn id="4" xr3:uid="{E99F4D16-1AFB-4115-A8C2-92F4F12E75F0}" name="# total Qs" dataDxfId="73"/>
+    <tableColumn id="7" xr3:uid="{D4124943-F8BF-4815-B6B9-91C683C8A94C}" name="# Solved Qs" dataDxfId="72"/>
+    <tableColumn id="5" xr3:uid="{6A1CC701-3B3F-48D6-A63E-0D0D28D38855}" name="Ranking" dataDxfId="71"/>
+    <tableColumn id="6" xr3:uid="{2DF92217-CA09-48F3-B4F6-01C752A7709A}" name="Are remainings solved ?" dataDxfId="70"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{C7ACFC98-5037-44D8-82A3-B31E6683EF89}" name="Table510" displayName="Table510" ref="C4:F15" totalsRowShown="0" headerRowDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{C7ACFC98-5037-44D8-82A3-B31E6683EF89}" name="Table510" displayName="Table510" ref="C4:F15" totalsRowShown="0" headerRowDxfId="69">
   <autoFilter ref="C4:F15" xr:uid="{C7ACFC98-5037-44D8-82A3-B31E6683EF89}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{38FEAE95-18E2-4FE0-BD6A-9BE906D4AFCC}" name="Sr. No." dataDxfId="53"/>
-    <tableColumn id="2" xr3:uid="{515E0F35-8C77-4BD4-99B5-16D2F593FC0D}" name="Project name" dataDxfId="52"/>
-    <tableColumn id="3" xr3:uid="{ED1A562C-F12C-46A6-A207-873D0289DC8F}" name="Skills used " dataDxfId="51"/>
-    <tableColumn id="4" xr3:uid="{484475D7-C606-4DEC-88C4-3D78EDF74E20}" name="Notes about it" dataDxfId="50"/>
+    <tableColumn id="1" xr3:uid="{38FEAE95-18E2-4FE0-BD6A-9BE906D4AFCC}" name="Sr. No." dataDxfId="68"/>
+    <tableColumn id="2" xr3:uid="{515E0F35-8C77-4BD4-99B5-16D2F593FC0D}" name="Project name" dataDxfId="67"/>
+    <tableColumn id="3" xr3:uid="{ED1A562C-F12C-46A6-A207-873D0289DC8F}" name="Skills used " dataDxfId="66"/>
+    <tableColumn id="4" xr3:uid="{484475D7-C606-4DEC-88C4-3D78EDF74E20}" name="Notes about it" dataDxfId="65"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{F04800D1-1296-49C2-9C89-FF4D36C3C5FA}" name="Table51011" displayName="Table51011" ref="C4:F15" totalsRowShown="0" headerRowDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{F04800D1-1296-49C2-9C89-FF4D36C3C5FA}" name="Table51011" displayName="Table51011" ref="C4:F15" totalsRowShown="0" headerRowDxfId="64">
   <autoFilter ref="C4:F15" xr:uid="{F04800D1-1296-49C2-9C89-FF4D36C3C5FA}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{75C622E8-8C93-498B-BB53-4AB82294F580}" name="Sr. No." dataDxfId="48"/>
-    <tableColumn id="2" xr3:uid="{491A9B10-7CCF-4151-BC22-1F881029D1CF}" name="Book name" dataDxfId="47"/>
-    <tableColumn id="3" xr3:uid="{79454B67-6983-4C7D-8F1A-1ABD4C8AA5EB}" name="Author " dataDxfId="46"/>
-    <tableColumn id="4" xr3:uid="{9F631DF3-35C9-4F10-AAF7-8FC855753250}" name="Learnings" dataDxfId="45"/>
+    <tableColumn id="1" xr3:uid="{75C622E8-8C93-498B-BB53-4AB82294F580}" name="Sr. No." dataDxfId="63"/>
+    <tableColumn id="2" xr3:uid="{491A9B10-7CCF-4151-BC22-1F881029D1CF}" name="Book name" dataDxfId="62"/>
+    <tableColumn id="3" xr3:uid="{79454B67-6983-4C7D-8F1A-1ABD4C8AA5EB}" name="Author " dataDxfId="61"/>
+    <tableColumn id="4" xr3:uid="{9F631DF3-35C9-4F10-AAF7-8FC855753250}" name="Learnings" dataDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FA275680-42C1-4CF5-9E62-42189E8A54FD}" name="Table1" displayName="Table1" ref="B72:F81" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FA275680-42C1-4CF5-9E62-42189E8A54FD}" name="Table1" displayName="Table1" ref="B72:F81" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
   <autoFilter ref="B72:F81" xr:uid="{FA275680-42C1-4CF5-9E62-42189E8A54FD}"/>
   <tableColumns count="5">
-    <tableColumn id="2" xr3:uid="{983B3321-F8D6-4B25-9AC8-187F8F3D33CC}" name="Sr. No." dataDxfId="95"/>
-    <tableColumn id="3" xr3:uid="{F86F5107-9EFE-4314-969C-E6DCD9A59B13}" name="Priority" dataDxfId="94"/>
-    <tableColumn id="4" xr3:uid="{7768FE33-8E07-4F5D-B874-306D7FC0ACB4}" name="Segment" dataDxfId="93"/>
-    <tableColumn id="5" xr3:uid="{AA766249-D3BA-403B-8A4B-9D3CB0E8DDF6}" name="Notes" dataDxfId="92"/>
-    <tableColumn id="6" xr3:uid="{DC096C63-8440-4369-AFCD-C38D5E75FDB4}" name="Status" dataDxfId="91"/>
+    <tableColumn id="2" xr3:uid="{983B3321-F8D6-4B25-9AC8-187F8F3D33CC}" name="Sr. No." dataDxfId="57"/>
+    <tableColumn id="3" xr3:uid="{F86F5107-9EFE-4314-969C-E6DCD9A59B13}" name="Priority" dataDxfId="56"/>
+    <tableColumn id="4" xr3:uid="{7768FE33-8E07-4F5D-B874-306D7FC0ACB4}" name="Segment" dataDxfId="55"/>
+    <tableColumn id="5" xr3:uid="{AA766249-D3BA-403B-8A4B-9D3CB0E8DDF6}" name="Notes" dataDxfId="54"/>
+    <tableColumn id="6" xr3:uid="{DC096C63-8440-4369-AFCD-C38D5E75FDB4}" name="Status" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6875C3DB-155D-480E-87DC-9FFB83877AE4}" name="Table134" displayName="Table134" ref="C8:E22" totalsRowShown="0" headerRowDxfId="90">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6875C3DB-155D-480E-87DC-9FFB83877AE4}" name="Table134" displayName="Table134" ref="C8:E22" totalsRowShown="0" headerRowDxfId="52">
   <autoFilter ref="C8:E22" xr:uid="{6875C3DB-155D-480E-87DC-9FFB83877AE4}"/>
   <tableColumns count="3">
-    <tableColumn id="2" xr3:uid="{D58BACB9-C929-4657-A941-1C7BCD578EDF}" name="Sr. No." dataDxfId="89"/>
-    <tableColumn id="3" xr3:uid="{2C6EBFA5-520C-473D-BBAC-0D5F31F4B191}" name="Segments" dataDxfId="88"/>
-    <tableColumn id="6" xr3:uid="{369550EE-78CE-4F66-875F-F34D301E4A0E}" name="Status" dataDxfId="87"/>
+    <tableColumn id="2" xr3:uid="{D58BACB9-C929-4657-A941-1C7BCD578EDF}" name="Sr. No." dataDxfId="51"/>
+    <tableColumn id="3" xr3:uid="{2C6EBFA5-520C-473D-BBAC-0D5F31F4B191}" name="Segments" dataDxfId="50"/>
+    <tableColumn id="6" xr3:uid="{369550EE-78CE-4F66-875F-F34D301E4A0E}" name="Status" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{788F11B4-6638-437A-BA2F-755567F822A6}" name="Table1345" displayName="Table1345" ref="C27:E67" totalsRowShown="0" headerRowDxfId="86">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{788F11B4-6638-437A-BA2F-755567F822A6}" name="Table1345" displayName="Table1345" ref="C27:E67" totalsRowShown="0" headerRowDxfId="48">
   <autoFilter ref="C27:E67" xr:uid="{788F11B4-6638-437A-BA2F-755567F822A6}"/>
   <tableColumns count="3">
-    <tableColumn id="5" xr3:uid="{760912DC-252C-490D-ABB6-BB7CFB907BE3}" name="Sr. No." dataDxfId="85"/>
-    <tableColumn id="1" xr3:uid="{7CB8FDA8-DE34-41AD-A040-9BC8A65E7DD5}" name="Segment" dataDxfId="84"/>
-    <tableColumn id="6" xr3:uid="{528137CC-3CA7-445D-8720-7662B0C9A622}" name="Status" dataDxfId="83"/>
+    <tableColumn id="5" xr3:uid="{760912DC-252C-490D-ABB6-BB7CFB907BE3}" name="Sr. No." dataDxfId="47"/>
+    <tableColumn id="1" xr3:uid="{7CB8FDA8-DE34-41AD-A040-9BC8A65E7DD5}" name="Segment" dataDxfId="46"/>
+    <tableColumn id="6" xr3:uid="{528137CC-3CA7-445D-8720-7662B0C9A622}" name="Status" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2018,22 +2045,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:15" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="4" spans="1:15" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
@@ -2333,22 +2360,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F3" s="2"/>
@@ -2419,10 +2446,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8060A9B2-7BC5-4235-86F0-815C6E85C7CC}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.77734375" defaultRowHeight="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2436,22 +2463,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F3" s="2"/>
@@ -2484,8 +2511,8 @@
       <c r="C5" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="D5" s="10">
-        <v>2</v>
+      <c r="D5" s="12" t="s">
+        <v>128</v>
       </c>
       <c r="E5" s="2"/>
     </row>
@@ -2499,8 +2526,8 @@
       <c r="C6" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="D6" s="10">
-        <v>1</v>
+      <c r="D6" s="10" t="s">
+        <v>126</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -2514,8 +2541,8 @@
       <c r="C7" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="D7" s="10">
-        <v>1</v>
+      <c r="D7" s="10" t="s">
+        <v>126</v>
       </c>
       <c r="E7" s="2"/>
     </row>
@@ -2529,8 +2556,8 @@
       <c r="C8" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="D8" s="10">
-        <v>1</v>
+      <c r="D8" s="10" t="s">
+        <v>135</v>
       </c>
       <c r="E8" s="2"/>
     </row>
@@ -2544,8 +2571,8 @@
       <c r="C9" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="D9" s="10">
-        <v>1</v>
+      <c r="D9" s="10" t="s">
+        <v>136</v>
       </c>
       <c r="E9" s="2"/>
     </row>
@@ -2559,45 +2586,99 @@
       <c r="C10" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="D10" s="10">
-        <v>1</v>
+      <c r="D10" s="10" t="s">
+        <v>135</v>
       </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:6" s="11" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
+      <c r="A11" s="10">
+        <v>7</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>137</v>
+      </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:6" s="11" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
+      <c r="A12" s="10">
+        <v>8</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>128</v>
+      </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:6" s="11" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
+      <c r="A13" s="10">
+        <v>9</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>126</v>
+      </c>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:6" s="11" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
+      <c r="A14" s="10">
+        <v>10</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>138</v>
+      </c>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:6" s="11" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
+      <c r="A15" s="10">
+        <v>11</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>137</v>
+      </c>
       <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" s="11" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" s="11" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2629,24 +2710,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
     </row>
     <row r="2" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
     </row>
     <row r="3" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G3" s="2"/>
@@ -2736,26 +2817,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
     </row>
     <row r="2" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="3" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H3" s="2"/>
@@ -2802,26 +2883,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
     </row>
     <row r="2" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="3" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H3" s="2"/>
@@ -2855,8 +2936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA808F5-CFD7-47C2-A961-FADC6CC1CBFE}">
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="F76" sqref="F76"/>
+    <sheetView showGridLines="0" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2870,52 +2951,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
     </row>
     <row r="2" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
     </row>
     <row r="3" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
     </row>
     <row r="6" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
     </row>
     <row r="7" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
     </row>
     <row r="8" spans="1:8" s="6" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="7"/>
@@ -3095,20 +3176,20 @@
       <c r="F22"/>
     </row>
     <row r="25" spans="2:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
     </row>
     <row r="26" spans="2:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
     </row>
     <row r="27" spans="2:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C27" s="7" t="s">
@@ -3576,20 +3657,20 @@
       <c r="F67"/>
     </row>
     <row r="70" spans="2:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="13" t="s">
+      <c r="B70" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C70" s="13"/>
-      <c r="D70" s="13"/>
-      <c r="E70" s="13"/>
-      <c r="F70" s="13"/>
+      <c r="C70" s="15"/>
+      <c r="D70" s="15"/>
+      <c r="E70" s="15"/>
+      <c r="F70" s="15"/>
     </row>
     <row r="71" spans="2:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="13"/>
-      <c r="C71" s="13"/>
-      <c r="D71" s="13"/>
-      <c r="E71" s="13"/>
-      <c r="F71" s="13"/>
+      <c r="B71" s="15"/>
+      <c r="C71" s="15"/>
+      <c r="D71" s="15"/>
+      <c r="E71" s="15"/>
+      <c r="F71" s="15"/>
     </row>
     <row r="72" spans="2:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B72" s="7" t="s">
@@ -3787,26 +3868,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
     </row>
     <row r="2" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="3" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H3" s="2"/>
@@ -3961,26 +4042,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
     </row>
     <row r="2" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="3" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H3" s="2"/>

</xml_diff>

<commit_message>
Updating Schedule and daily tasks
</commit_message>
<xml_diff>
--- a/Master-Sheet.xlsx
+++ b/Master-Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OTHERS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D6A635-1398-4FC8-8A3D-87F2DA52C138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A4CBDA-643B-4837-8C8C-EB298E38BDCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="702" xr2:uid="{0042A21B-FF33-4EBF-B65C-49274797135A}"/>
+    <workbookView xWindow="4500" yWindow="3360" windowWidth="17280" windowHeight="8880" tabRatio="702" xr2:uid="{0042A21B-FF33-4EBF-B65C-49274797135A}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily" sheetId="10" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="143">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -246,12 +246,6 @@
     <t>Segment</t>
   </si>
   <si>
-    <t>Complete HTML</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Propositions and 1st order logic - DM </t>
-  </si>
-  <si>
     <t>Complete 10 points on Arcade</t>
   </si>
   <si>
@@ -463,6 +457,12 @@
   </si>
   <si>
     <t>Start Arcade with 2 mail ID</t>
+  </si>
+  <si>
+    <t>Assigned</t>
+  </si>
+  <si>
+    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -2042,8 +2042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA808F5-CFD7-47C2-A961-FADC6CC1CBFE}">
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="E80" sqref="E80"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="F77" sqref="F77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2124,7 +2124,7 @@
         <v>54</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>25</v>
+        <v>141</v>
       </c>
       <c r="F9"/>
     </row>
@@ -2314,7 +2314,7 @@
         <v>1</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>25</v>
@@ -2326,7 +2326,7 @@
         <v>2</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>25</v>
@@ -2338,7 +2338,7 @@
         <v>4</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>25</v>
@@ -2350,7 +2350,7 @@
         <v>5</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>25</v>
@@ -2362,7 +2362,7 @@
         <v>6</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>25</v>
@@ -2374,7 +2374,7 @@
         <v>7</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>25</v>
@@ -2386,7 +2386,7 @@
         <v>8</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>25</v>
@@ -2398,7 +2398,7 @@
         <v>9</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>25</v>
@@ -2410,7 +2410,7 @@
         <v>10</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>25</v>
@@ -2422,7 +2422,7 @@
         <v>11</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>25</v>
@@ -2434,7 +2434,7 @@
         <v>12</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>25</v>
@@ -2446,7 +2446,7 @@
         <v>13</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>25</v>
@@ -2458,7 +2458,7 @@
         <v>14</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>25</v>
@@ -2470,7 +2470,7 @@
         <v>15</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>25</v>
@@ -2485,7 +2485,7 @@
         <v>16</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>25</v>
@@ -2497,7 +2497,7 @@
         <v>17</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>25</v>
@@ -2509,7 +2509,7 @@
         <v>18</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>25</v>
@@ -2521,7 +2521,7 @@
         <v>19</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>25</v>
@@ -2533,7 +2533,7 @@
         <v>20</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>25</v>
@@ -2545,7 +2545,7 @@
         <v>21</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>25</v>
@@ -2557,7 +2557,7 @@
         <v>22</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>25</v>
@@ -2569,7 +2569,7 @@
         <v>23</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>25</v>
@@ -2581,7 +2581,7 @@
         <v>24</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>25</v>
@@ -2593,7 +2593,7 @@
         <v>25</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>25</v>
@@ -2605,7 +2605,7 @@
         <v>26</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>25</v>
@@ -2617,7 +2617,7 @@
         <v>27</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>25</v>
@@ -2629,7 +2629,7 @@
         <v>28</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>25</v>
@@ -2641,7 +2641,7 @@
         <v>29</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>25</v>
@@ -2653,7 +2653,7 @@
         <v>30</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>25</v>
@@ -2665,7 +2665,7 @@
         <v>31</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>25</v>
@@ -2677,7 +2677,7 @@
         <v>32</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>25</v>
@@ -2689,7 +2689,7 @@
         <v>33</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>25</v>
@@ -2701,7 +2701,7 @@
         <v>34</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>25</v>
@@ -2713,7 +2713,7 @@
         <v>35</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>25</v>
@@ -2725,7 +2725,7 @@
         <v>36</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>25</v>
@@ -2740,10 +2740,10 @@
         <v>37</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>25</v>
+        <v>142</v>
       </c>
       <c r="F65"/>
     </row>
@@ -2752,7 +2752,7 @@
         <v>38</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>25</v>
@@ -2803,10 +2803,10 @@
         <v>26</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>70</v>
+        <v>107</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>25</v>
+        <v>106</v>
       </c>
     </row>
     <row r="74" spans="2:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -2817,7 +2817,7 @@
         <v>26</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>71</v>
+        <v>138</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>25</v>
@@ -2828,13 +2828,13 @@
         <v>3</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>109</v>
+        <v>70</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="76" spans="2:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -2845,10 +2845,10 @@
         <v>27</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="77" spans="2:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -2856,13 +2856,13 @@
         <v>5</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>27</v>
+        <v>139</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>108</v>
+        <v>25</v>
       </c>
     </row>
     <row r="78" spans="2:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -2873,7 +2873,7 @@
         <v>26</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>25</v>
@@ -2883,12 +2883,7 @@
       <c r="B79" s="2">
         <v>7</v>
       </c>
-      <c r="C79" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D79" s="9" t="s">
-        <v>139</v>
-      </c>
+      <c r="D79" s="9"/>
       <c r="F79" s="2" t="s">
         <v>25</v>
       </c>
@@ -2897,17 +2892,15 @@
       <c r="B80" s="2">
         <v>8</v>
       </c>
-      <c r="C80" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="D80" s="9" t="s">
-        <v>142</v>
-      </c>
+      <c r="D80" s="9"/>
       <c r="F80" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="81" spans="4:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B81" s="2">
+        <v>9</v>
+      </c>
       <c r="D81" s="9"/>
       <c r="F81" s="2" t="s">
         <v>25</v>
@@ -3114,7 +3107,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>2</v>
@@ -3123,7 +3116,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>5</v>
@@ -3137,13 +3130,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="3"/>
@@ -3157,13 +3150,13 @@
         <v>7</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -3175,13 +3168,13 @@
         <v>9</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
@@ -3199,13 +3192,13 @@
         <v>26</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -3217,13 +3210,13 @@
         <v>1009</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:15" s="11" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.35">
@@ -3417,7 +3410,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
@@ -3459,13 +3452,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E5" s="2"/>
     </row>
@@ -3474,13 +3467,13 @@
         <v>2</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -3489,13 +3482,13 @@
         <v>3</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E7" s="2"/>
     </row>
@@ -3504,13 +3497,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E8" s="2"/>
     </row>
@@ -3519,13 +3512,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E9" s="2"/>
     </row>
@@ -3534,13 +3527,13 @@
         <v>6</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E10" s="2"/>
     </row>
@@ -3549,13 +3542,13 @@
         <v>7</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E11" s="2"/>
     </row>
@@ -3564,13 +3557,13 @@
         <v>8</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E12" s="2"/>
     </row>
@@ -3579,13 +3572,13 @@
         <v>9</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E13" s="2"/>
     </row>
@@ -3594,13 +3587,13 @@
         <v>10</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E14" s="2"/>
     </row>
@@ -3609,13 +3602,13 @@
         <v>11</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E15" s="2"/>
     </row>

</xml_diff>